<commit_message>
Update Kho gửi phòng sxbh 11_2025.xlsx
</commit_message>
<xml_diff>
--- a/5.Other/Thiết bị kho gửi/2025/Kho gửi phòng sxbh 11_2025.xlsx
+++ b/5.Other/Thiết bị kho gửi/2025/Kho gửi phòng sxbh 11_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNET\5.Other\Thiết bị kho gửi\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B9C72B-C97A-44DD-8CAA-8C3EF2143BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4FC050-B9EF-4D96-95C3-832FFAFA12A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nhập xuất tồn" sheetId="1" r:id="rId1"/>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,15 +595,15 @@
       </c>
       <c r="E5" s="3">
         <f>Xuất!AH6+'Hủy tb'!AH6</f>
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" ref="F5:F6" si="0">C5+D5-E5</f>
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="H5" s="1">
         <f>F5-G5</f>
-        <v>95</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1755,8 +1755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AH19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2008,7 +2008,9 @@
         <v>2</v>
       </c>
       <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="H6" s="8">
+        <v>48</v>
+      </c>
       <c r="I6" s="8"/>
       <c r="J6" s="7"/>
       <c r="K6" s="8"/>
@@ -2036,7 +2038,7 @@
       <c r="AG6" s="8"/>
       <c r="AH6" s="8">
         <f t="shared" ref="AH6:AH19" si="0">SUM(C6:AG6)</f>
-        <v>23</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">

</xml_diff>